<commit_message>
add square mass import usa, add skus to data
</commit_message>
<xml_diff>
--- a/normalized-data/square-mass-import-catalog_template.xlsx
+++ b/normalized-data/square-mass-import-catalog_template.xlsx
@@ -233,6 +233,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -253,24 +254,28 @@
       <sz val="12"/>
       <name val="Verdana"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="14"/>
       <name val="Verdana"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
       <sz val="12"/>
       <name val="Verdana"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="12"/>
       <name val="Verdana"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -326,35 +331,35 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -435,22 +440,46 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:AF6"/>
+  <dimension ref="A2:AF108"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AF100" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7:AQ108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="13.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="3" style="2" width="13.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="3" width="13.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="13.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="23" style="2" width="13.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="25" style="1" width="13.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="28" style="2" width="13.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="30" style="1" width="13.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="34.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="22.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="16.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="20.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="10.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="36.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="101.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="30.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="62.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="18.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="37.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="2" width="94.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="2" width="15.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="2" width="29.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="2" width="38.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="22.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="2" width="36.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="2" width="22.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="2" width="20.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="3" width="7.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="22.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="2" width="11.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="2" width="13.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="33.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="20.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="19.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="2" width="39.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="2" width="35.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="1" width="43.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="1" width="40.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="30.64"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -723,6 +752,411 @@
         <v>55</v>
       </c>
     </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G7" s="1"/>
+      <c r="U7" s="1"/>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G8" s="1"/>
+      <c r="U8" s="1"/>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G9" s="1"/>
+      <c r="U9" s="1"/>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G10" s="1"/>
+      <c r="U10" s="1"/>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G11" s="1"/>
+      <c r="U11" s="1"/>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G12" s="1"/>
+      <c r="U12" s="1"/>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G13" s="1"/>
+      <c r="U13" s="1"/>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G14" s="1"/>
+      <c r="U14" s="1"/>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G15" s="1"/>
+      <c r="U15" s="1"/>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G16" s="1"/>
+      <c r="U16" s="1"/>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G17" s="1"/>
+      <c r="U17" s="1"/>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G18" s="1"/>
+      <c r="U18" s="1"/>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G19" s="1"/>
+      <c r="U19" s="1"/>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G20" s="1"/>
+      <c r="U20" s="1"/>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G21" s="1"/>
+      <c r="U21" s="1"/>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G22" s="1"/>
+      <c r="U22" s="1"/>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G23" s="1"/>
+      <c r="U23" s="1"/>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G24" s="1"/>
+      <c r="U24" s="1"/>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G25" s="1"/>
+      <c r="U25" s="1"/>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G26" s="1"/>
+      <c r="U26" s="1"/>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G27" s="1"/>
+      <c r="U27" s="1"/>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G28" s="1"/>
+      <c r="U28" s="1"/>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G29" s="1"/>
+      <c r="U29" s="1"/>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G30" s="1"/>
+      <c r="U30" s="1"/>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G31" s="1"/>
+      <c r="U31" s="1"/>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G32" s="1"/>
+      <c r="U32" s="1"/>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G33" s="1"/>
+      <c r="U33" s="1"/>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G34" s="1"/>
+      <c r="U34" s="1"/>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G35" s="1"/>
+      <c r="U35" s="1"/>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G36" s="1"/>
+      <c r="U36" s="1"/>
+    </row>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G37" s="1"/>
+      <c r="U37" s="1"/>
+    </row>
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G38" s="1"/>
+      <c r="U38" s="1"/>
+    </row>
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G39" s="1"/>
+      <c r="U39" s="1"/>
+    </row>
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G40" s="1"/>
+      <c r="U40" s="1"/>
+    </row>
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G41" s="1"/>
+      <c r="U41" s="1"/>
+    </row>
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G42" s="1"/>
+      <c r="U42" s="1"/>
+    </row>
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G43" s="1"/>
+      <c r="U43" s="1"/>
+    </row>
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G44" s="1"/>
+      <c r="U44" s="1"/>
+    </row>
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G45" s="1"/>
+      <c r="U45" s="1"/>
+    </row>
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G46" s="1"/>
+      <c r="U46" s="1"/>
+    </row>
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G47" s="1"/>
+      <c r="U47" s="1"/>
+    </row>
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G48" s="1"/>
+      <c r="U48" s="1"/>
+    </row>
+    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G49" s="1"/>
+      <c r="U49" s="1"/>
+    </row>
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G50" s="1"/>
+      <c r="U50" s="1"/>
+    </row>
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G51" s="1"/>
+      <c r="U51" s="1"/>
+    </row>
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G52" s="1"/>
+      <c r="U52" s="1"/>
+    </row>
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G53" s="1"/>
+      <c r="U53" s="1"/>
+    </row>
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G54" s="1"/>
+      <c r="U54" s="1"/>
+    </row>
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G55" s="1"/>
+      <c r="U55" s="1"/>
+    </row>
+    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G56" s="1"/>
+      <c r="U56" s="1"/>
+    </row>
+    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G57" s="1"/>
+      <c r="U57" s="1"/>
+    </row>
+    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G58" s="1"/>
+      <c r="U58" s="1"/>
+    </row>
+    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G59" s="1"/>
+      <c r="U59" s="1"/>
+    </row>
+    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G60" s="1"/>
+      <c r="U60" s="1"/>
+    </row>
+    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G61" s="1"/>
+      <c r="U61" s="1"/>
+    </row>
+    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G62" s="1"/>
+      <c r="U62" s="1"/>
+    </row>
+    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G63" s="1"/>
+      <c r="U63" s="1"/>
+    </row>
+    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G64" s="1"/>
+      <c r="U64" s="1"/>
+    </row>
+    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G65" s="1"/>
+      <c r="U65" s="1"/>
+    </row>
+    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G66" s="1"/>
+      <c r="U66" s="1"/>
+    </row>
+    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G67" s="1"/>
+      <c r="U67" s="1"/>
+    </row>
+    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G68" s="1"/>
+      <c r="U68" s="1"/>
+    </row>
+    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G69" s="1"/>
+      <c r="U69" s="1"/>
+    </row>
+    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G70" s="1"/>
+      <c r="U70" s="1"/>
+    </row>
+    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G71" s="1"/>
+      <c r="U71" s="1"/>
+    </row>
+    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G72" s="1"/>
+      <c r="U72" s="1"/>
+    </row>
+    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G73" s="1"/>
+      <c r="U73" s="1"/>
+    </row>
+    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G74" s="1"/>
+      <c r="U74" s="1"/>
+    </row>
+    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G75" s="1"/>
+      <c r="U75" s="1"/>
+    </row>
+    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G76" s="1"/>
+      <c r="U76" s="1"/>
+    </row>
+    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G77" s="1"/>
+      <c r="U77" s="1"/>
+    </row>
+    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G78" s="1"/>
+      <c r="U78" s="1"/>
+    </row>
+    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G79" s="1"/>
+      <c r="U79" s="1"/>
+    </row>
+    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G80" s="1"/>
+      <c r="U80" s="1"/>
+    </row>
+    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G81" s="1"/>
+      <c r="U81" s="1"/>
+    </row>
+    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G82" s="1"/>
+      <c r="U82" s="1"/>
+    </row>
+    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G83" s="1"/>
+      <c r="U83" s="1"/>
+    </row>
+    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G84" s="1"/>
+      <c r="U84" s="1"/>
+    </row>
+    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G85" s="1"/>
+      <c r="U85" s="1"/>
+    </row>
+    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G86" s="1"/>
+      <c r="U86" s="1"/>
+    </row>
+    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G87" s="1"/>
+      <c r="U87" s="1"/>
+    </row>
+    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G88" s="1"/>
+      <c r="U88" s="1"/>
+    </row>
+    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G89" s="1"/>
+      <c r="U89" s="1"/>
+    </row>
+    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G90" s="1"/>
+      <c r="U90" s="1"/>
+    </row>
+    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G91" s="1"/>
+      <c r="U91" s="1"/>
+    </row>
+    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G92" s="1"/>
+      <c r="U92" s="1"/>
+    </row>
+    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G93" s="1"/>
+      <c r="U93" s="1"/>
+    </row>
+    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G94" s="1"/>
+      <c r="U94" s="1"/>
+    </row>
+    <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G95" s="1"/>
+      <c r="U95" s="1"/>
+    </row>
+    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G96" s="1"/>
+      <c r="U96" s="1"/>
+    </row>
+    <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G97" s="1"/>
+      <c r="U97" s="1"/>
+    </row>
+    <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G98" s="1"/>
+      <c r="U98" s="1"/>
+    </row>
+    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G99" s="1"/>
+      <c r="U99" s="1"/>
+    </row>
+    <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G100" s="1"/>
+      <c r="U100" s="1"/>
+    </row>
+    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G101" s="1"/>
+      <c r="U101" s="1"/>
+    </row>
+    <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G102" s="1"/>
+      <c r="U102" s="1"/>
+    </row>
+    <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G103" s="1"/>
+      <c r="U103" s="1"/>
+    </row>
+    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G104" s="1"/>
+      <c r="U104" s="1"/>
+    </row>
+    <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G105" s="1"/>
+      <c r="U105" s="1"/>
+    </row>
+    <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G106" s="1"/>
+      <c r="U106" s="1"/>
+    </row>
+    <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G107" s="1"/>
+      <c r="U107" s="1"/>
+    </row>
+    <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A2:D2"/>
@@ -746,7 +1180,7 @@
   <dimension ref="A2:I2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A7:AQ108 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>